<commit_message>
new terms of trade data from OECD and IMF and credit default swap data (CDS)
</commit_message>
<xml_diff>
--- a/input/_var_description.xlsx
+++ b/input/_var_description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktor\Dropbox\GitHub\macroX_sovereign-yield-spreads\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2E7DD20-0027-4CE3-87D9-8FF388FE718B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563EBE6A-B593-4106-B7A8-3587388FD2B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12030" yWindow="2805" windowWidth="14865" windowHeight="11820" xr2:uid="{3668E29E-1E2B-4ADB-8261-C81CCA08E4FC}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{3668E29E-1E2B-4ADB-8261-C81CCA08E4FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t>var name in R</t>
   </si>
@@ -92,9 +92,6 @@
     <t>trade balance</t>
   </si>
   <si>
-    <t>tot</t>
-  </si>
-  <si>
     <t>terms of trade (not the same index across countries?)</t>
   </si>
   <si>
@@ -192,6 +189,27 @@
   </si>
   <si>
     <t>propensity to invest in risky bonds, the higher, if spread for risky US corporate bonds (baa) over US treasuries increases, then market participants less willing to invest in risky bonds (higher baa yield for incentivizing them to do so), therefore higher corporate bond spreads supposed to lead to higher sovereign yield spreads</t>
+  </si>
+  <si>
+    <t>tot_eiu</t>
+  </si>
+  <si>
+    <t>tot_oecd</t>
+  </si>
+  <si>
+    <t>same, but retrieved from OECD database, since data from economist intelligence unit is indexed weirdly (index years are different) - OECD omits malta and cyprus though, but shouldn't matter too much</t>
+  </si>
+  <si>
+    <t>tot_imf</t>
+  </si>
+  <si>
+    <t>terms of trade</t>
+  </si>
+  <si>
+    <t>terms of trade (malta, cyprus missing)</t>
+  </si>
+  <si>
+    <t>same, own calculation (see terms_of_trade_IMF.xlsx), export/import price indices according to IMF weighted by ratio of exports/imports to GDP - should be fine, I guess</t>
   </si>
 </sst>
 </file>
@@ -561,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D22546-088C-4F62-9A44-326BBEB3FE91}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,13 +597,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -604,10 +622,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -618,10 +636,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
         <v>36</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -632,10 +650,10 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -646,10 +664,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -660,10 +678,10 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -674,10 +692,10 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -688,10 +706,10 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -702,101 +720,123 @@
         <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
         <v>44</v>
-      </c>
-      <c r="D10" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>47</v>
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" t="s">
-        <v>48</v>
+      <c r="A15" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
         <v>24</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="C16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>27</v>
       </c>
-      <c r="C19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added real effective exchange rate and EMU membership
</commit_message>
<xml_diff>
--- a/input/_var_description.xlsx
+++ b/input/_var_description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktor\Dropbox\GitHub\macroX_sovereign-yield-spreads\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCA0AA0-DEE1-4BA7-979C-0A04A7AE6ADE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32485358-F87D-4188-B85B-A71F6EAC6175}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{3668E29E-1E2B-4ADB-8261-C81CCA08E4FC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
   <si>
     <t>var name in R</t>
   </si>
@@ -219,6 +219,24 @@
   </si>
   <si>
     <t>indicator for credit risk and likelihood of default for a country, should in my opinion be highly important - questionable if we should include it though, because in theory cds should actually be determined by the other explanatory variables</t>
+  </si>
+  <si>
+    <t>emu</t>
+  </si>
+  <si>
+    <t>EMU membership</t>
+  </si>
+  <si>
+    <t>reer</t>
+  </si>
+  <si>
+    <t>real effective exchange rate</t>
+  </si>
+  <si>
+    <t>not sure, yet to think about it</t>
+  </si>
+  <si>
+    <t>probably convergence in spreads should take place because investors wanna invest in euros</t>
   </si>
 </sst>
 </file>
@@ -588,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D22546-088C-4F62-9A44-326BBEB3FE91}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,83 +803,108 @@
         <v>61</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
         <v>32</v>
       </c>
       <c r="D19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>26</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>35</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" t="s">
         <v>35</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D25" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>